<commit_message>
elec category import purpose
elec category import purpose
</commit_message>
<xml_diff>
--- a/uploads/Electroniccategoryfile.xlsx
+++ b/uploads/Electroniccategoryfile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>sno</t>
   </si>
@@ -72,24 +72,6 @@
     <t>Product description</t>
   </si>
   <si>
-    <t>otherunique</t>
-  </si>
-  <si>
-    <t>prodctname</t>
-  </si>
-  <si>
-    <t>999</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>metakeyword</t>
-  </si>
-  <si>
-    <t>meta tile</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -105,9 +87,6 @@
     <t>4gb,500gb</t>
   </si>
   <si>
-    <t>55555</t>
-  </si>
-  <si>
     <t>Offers</t>
   </si>
   <si>
@@ -153,9 +132,6 @@
     <t>Product image12</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -171,10 +147,16 @@
     <t>Ideal for</t>
   </si>
   <si>
-    <t>ideal for</t>
-  </si>
-  <si>
     <t>elect</t>
+  </si>
+  <si>
+    <t>Elec</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -525,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -571,10 +553,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>14</v>
@@ -592,55 +574,55 @@
         <v>17</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -648,55 +630,37 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="Q2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="S2" t="s">
         <v>3</v>

</xml_diff>